<commit_message>
Added a project ZIP and teamwork defense generated data
</commit_message>
<xml_diff>
--- a/TeamAluminium/Output/Combined-Db-Report.xlsx
+++ b/TeamAluminium/Output/Combined-Db-Report.xlsx
@@ -32,334 +32,334 @@
     <t xml:space="preserve">Materials Layers</t>
   </si>
   <si>
+    <t xml:space="preserve">My Visionary Idealism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OilPainting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metaphysical Sky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WaxStatue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journey vs Head</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SprayPainting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geometric Dialogue with Momentary Echo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Pure Spirit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MetalSculpture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resignation and Absence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FrescoPainting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Interior of Innocence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nurse Deciphering the Artist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AcrylicPainting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unfolding Extracts from Autumnal Echo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PastelPainting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knowledge or Poetry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ephemeral Spirit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GlassSculpture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remixed Sister of Despair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reclining Peasant Rearranged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linear Singularity in 3 Stages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analysis and Cannibalism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dialogue with Reincarnated Disgust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emotional Idea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Philosophy of Fear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nudist Detaching the Composition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InkPainting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Context and Muse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StoneSculpture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pure Brushstroke of God</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peasant Deserting a Staircase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The False Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Meditative Journey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information or Context</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thing and Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tremulous Memories of High Expression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incidental Square</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My Departure of Fear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Cannibalism of Lust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Mystic Cannibalism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Song of War</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nothing of Fear - Composition VII</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transformation vs Sister</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stenographic Substance - Oversize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intuitive Brushstroke of Lust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Landscape with Fatal Future</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dialogue with Trapped Shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torqued Movement of Desire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peacock Deceiving the Canvas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Luminous Movement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silent Nurse (detail)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objective Path of Pain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fugue with Demoralized Expression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Sky of God</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manifesto of Silent Apropos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nude Decreasing the Orange Field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ode to Jumping Compound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purpose with Sadness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fugue with Intuitive Cannibalism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Three-Way Structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aphrodite or Projection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Element of Dreams 1955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extracts from Masked Limitation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Old Man Deceiving Humanism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nun Detaching a Staircase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nurse Desiring a Bureaucrat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sentiment with Reality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abstraction with Hope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Pataphysical Material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fragment of Autumnal Projection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drunk Bachelor - Composition VII</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Cannibalism of Innocence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work &amp; Edge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perceptive Boundry of Innocence</t>
+  </si>
+  <si>
     <t xml:space="preserve">Impression of Dying Image</t>
   </si>
   <si>
-    <t xml:space="preserve">MetalSculpture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Work &amp; Edge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InkPainting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Element of Dreams 1955</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AcrylicPainting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nurse Desiring a Bureaucrat</t>
+    <t xml:space="preserve">Luminous Rhubarb of Peace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seated Old Man (detail)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projection of Dreams (ironic)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perky Boy in Oil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absentminded Orpheus of Despair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stain and Work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virgin Deserting the Canvas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supposed Conflict of God</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complicated Stick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perceptive Eye - Number 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crying Virgin under Construction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Cannibalism of Death</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mechanical Literature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supposed Continuation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Act Including Interfering Lover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Religious Approach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masked Giraffe - Oversize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tender Aviator of Sorrow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virgin Descending the Left Corner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Idea of Dreams</t>
   </si>
   <si>
     <t xml:space="preserve">Reflecting Absence</t>
   </si>
   <si>
-    <t xml:space="preserve">FrescoPainting</t>
+    <t xml:space="preserve">Established Apparition of Demoralized Structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incidental Depth</t>
   </si>
   <si>
     <t xml:space="preserve">Nudist Desiring Humanism</t>
   </si>
   <si>
-    <t xml:space="preserve">WaxStatue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intuitive Brushstroke of Lust</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SprayPainting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drunk Bachelor - Composition VII</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OilPainting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Established Apparition of Demoralized Structure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resignation and Absence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Interior of Innocence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GlassSculpture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supposed Conflict of God</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luminous Rhubarb of Peace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Cannibalism of Lust</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Landscape with Fatal Future</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StoneSculpture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incidental Depth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abstraction with Hope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The False Information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Meditative Journey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Information or Context</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Pure Spirit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perceptive Eye - Number 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Sky of God</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tender Aviator of Sorrow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tremulous Memories of High Expression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ode to Jumping Compound</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Cannibalism of Innocence</t>
+    <t xml:space="preserve">The Absence of Lust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information of Desire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image and Painting</t>
   </si>
   <si>
     <t xml:space="preserve">Old Man Deserting Nature</t>
   </si>
   <si>
-    <t xml:space="preserve">Sentiment with Reality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Journey vs Head</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Context and Muse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perceptive Boundry of Innocence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Projection of Dreams (ironic)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crying Virgin under Construction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Pataphysical Material</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peasant Deserting a Staircase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Old Man Deceiving Humanism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PastelPainting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Complicated Stick</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geometric Dialogue with Momentary Echo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Virgin Descending the Left Corner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emotional Idea</t>
+    <t xml:space="preserve">Biblical Blob of Hate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pataphysical Nothing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface with Venus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extracts from Painted Air</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dialogue with Reflecting Summation</t>
   </si>
   <si>
     <t xml:space="preserve">Broken Component</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aphrodite or Projection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Absence of Lust</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Absentminded Orpheus of Despair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Song of War</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extracts from Masked Limitation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biblical Blob of Hate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nun Detaching a Staircase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manifesto of Silent Apropos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mechanical Literature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Mystic Cannibalism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Idea of Dreams</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metaphysical Sky</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pataphysical Nothing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Philosophy of Fear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fugue with Intuitive Cannibalism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">My Departure of Fear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Virgin Deserting the Canvas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transformation vs Sister</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perky Boy in Oil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Three-Way Structure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incidental Square</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peacock Deceiving the Canvas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dialogue with Reincarnated Disgust</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nurse Deciphering the Artist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nude Decreasing the Orange Field </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Religious Approach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Image and Painting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nudist Detaching the Composition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dialogue with Trapped Shape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Luminous Movement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ephemeral Spirit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purpose with Sadness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface with Venus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nothing of Fear - Composition VII</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thing and Design</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reclining Peasant Rearranged</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supposed Continuation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Knowledge or Poetry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unfolding Extracts from Autumnal Echo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fragment of Autumnal Projection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Information of Desire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silent Nurse (detail)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extracts from Painted Air</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stain and Work</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Masked Giraffe - Oversize</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stenographic Substance - Oversize</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linear Singularity in 3 Stages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Analysis and Cannibalism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pure Brushstroke of God</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remixed Sister of Despair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Cannibalism of Death</t>
-  </si>
-  <si>
-    <t xml:space="preserve">My Visionary Idealism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dialogue with Reflecting Summation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Objective Path of Pain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Torqued Movement of Desire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seated Old Man (detail)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fugue with Demoralized Expression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Act Including Interfering Lover</t>
   </si>
 </sst>
 </file>
@@ -437,10 +437,10 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>92.2</v>
+        <v>25.6</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -451,13 +451,13 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>3791090</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>53.8</v>
+        <v>74</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -471,10 +471,10 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>70.4</v>
+        <v>66.8</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -482,13 +482,13 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>9302597</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>22.9</v>
+        <v>92.6</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -505,10 +505,10 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>88.4</v>
+        <v>17.4</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -519,10 +519,10 @@
         <v>16</v>
       </c>
       <c r="C7">
-        <v>7662608</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>44.7</v>
+        <v>54.2</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -533,13 +533,13 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>34.4</v>
+        <v>47.1</v>
       </c>
       <c r="E8">
         <v>4</v>
@@ -547,36 +547,36 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
       <c r="C9">
-        <v>0</v>
+        <v>9237570</v>
       </c>
       <c r="D9">
-        <v>24.8</v>
+        <v>63.5</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
       <c r="C10">
-        <v>1975035</v>
+        <v>3594465</v>
       </c>
       <c r="D10">
-        <v>31.2</v>
+        <v>1.5</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -584,16 +584,16 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>5.5</v>
+        <v>12.6</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -604,10 +604,10 @@
         <v>24</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>6033705</v>
       </c>
       <c r="D12">
-        <v>54.7</v>
+        <v>59.5</v>
       </c>
       <c r="E12">
         <v>3</v>
@@ -618,16 +618,16 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C13">
-        <v>1796858</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>16.9</v>
+        <v>13.1</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -638,13 +638,13 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>6314887</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>80.9</v>
+        <v>83</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
@@ -652,16 +652,16 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C15">
-        <v>47621</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>82.6</v>
+        <v>10</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
@@ -669,13 +669,13 @@
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>66.3</v>
+        <v>22.4</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -683,70 +683,70 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>8646763</v>
       </c>
       <c r="D17">
-        <v>99.4</v>
+        <v>79.9</v>
       </c>
       <c r="E17">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>3526545</v>
       </c>
       <c r="D18">
-        <v>94.3</v>
+        <v>29.9</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <v>38.6</v>
+        <v>95.9</v>
       </c>
       <c r="E19">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
         <v>33</v>
       </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
       <c r="C20">
-        <v>9090932</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>85.1</v>
+        <v>32.5</v>
       </c>
       <c r="E20">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -754,115 +754,115 @@
         <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>7527686</v>
       </c>
       <c r="D21">
-        <v>96</v>
+        <v>59.6</v>
       </c>
       <c r="E21">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>6.1</v>
+        <v>83</v>
       </c>
       <c r="E22">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>6885901</v>
       </c>
       <c r="D23">
-        <v>17.5</v>
+        <v>25.5</v>
       </c>
       <c r="E23">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24">
-        <v>85.8</v>
+        <v>34.3</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>4531232</v>
       </c>
       <c r="D25">
-        <v>70.3</v>
+        <v>30.5</v>
       </c>
       <c r="E25">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26">
-        <v>84.1</v>
+        <v>41.1</v>
       </c>
       <c r="E26">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
       <c r="D27">
-        <v>32.6</v>
+        <v>20</v>
       </c>
       <c r="E27">
         <v>4</v>
@@ -870,58 +870,58 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C28">
-        <v>5767534</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>1.6</v>
+        <v>91.3</v>
       </c>
       <c r="E28">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
       <c r="D29">
-        <v>65.3</v>
+        <v>88.8</v>
       </c>
       <c r="E29">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30">
-        <v>54.5</v>
+        <v>2.8</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
@@ -930,7 +930,7 @@
         <v>0</v>
       </c>
       <c r="D31">
-        <v>39.2</v>
+        <v>5.8</v>
       </c>
       <c r="E31">
         <v>5</v>
@@ -938,7 +938,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
         <v>16</v>
@@ -947,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="D32">
-        <v>2.5</v>
+        <v>97.8</v>
       </c>
       <c r="E32">
         <v>5</v>
@@ -955,16 +955,16 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33">
-        <v>62.6</v>
+        <v>82</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -972,33 +972,33 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
-        <v>28.2</v>
+        <v>65.4</v>
       </c>
       <c r="E34">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
-        <v>76.7</v>
+        <v>25.8</v>
       </c>
       <c r="E35">
         <v>3</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B36" t="s">
         <v>16</v>
@@ -1015,24 +1015,24 @@
         <v>0</v>
       </c>
       <c r="D36">
-        <v>66</v>
+        <v>45.6</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <v>51.5</v>
+        <v>32.4</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -1040,19 +1040,19 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="C38">
-        <v>3947300</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>86.7</v>
+        <v>55.6</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
@@ -1060,13 +1060,13 @@
         <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
-        <v>92.4</v>
+        <v>48.6</v>
       </c>
       <c r="E39">
         <v>3</v>
@@ -1077,13 +1077,13 @@
         <v>54</v>
       </c>
       <c r="B40" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
-        <v>25.3</v>
+        <v>80.5</v>
       </c>
       <c r="E40">
         <v>2</v>
@@ -1094,16 +1094,16 @@
         <v>55</v>
       </c>
       <c r="B41" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41">
-        <v>48.5</v>
+        <v>33.2</v>
       </c>
       <c r="E41">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42">
@@ -1111,16 +1111,16 @@
         <v>56</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>5132597</v>
       </c>
       <c r="D42">
-        <v>44.5</v>
+        <v>8.3</v>
       </c>
       <c r="E42">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -1128,16 +1128,16 @@
         <v>57</v>
       </c>
       <c r="B43" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>5986675</v>
       </c>
       <c r="D43">
-        <v>10.9</v>
+        <v>29.5</v>
       </c>
       <c r="E43">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44">
@@ -1145,16 +1145,16 @@
         <v>58</v>
       </c>
       <c r="B44" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
       <c r="D44">
-        <v>6.8</v>
+        <v>12.9</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45">
@@ -1168,10 +1168,10 @@
         <v>0</v>
       </c>
       <c r="D45">
-        <v>94.7</v>
+        <v>10.1</v>
       </c>
       <c r="E45">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46">
@@ -1179,16 +1179,16 @@
         <v>60</v>
       </c>
       <c r="B46" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C46">
         <v>0</v>
       </c>
       <c r="D46">
-        <v>58.5</v>
+        <v>65.4</v>
       </c>
       <c r="E46">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -1196,13 +1196,13 @@
         <v>61</v>
       </c>
       <c r="B47" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C47">
         <v>0</v>
       </c>
       <c r="D47">
-        <v>6.5</v>
+        <v>17.5</v>
       </c>
       <c r="E47">
         <v>5</v>
@@ -1213,13 +1213,13 @@
         <v>62</v>
       </c>
       <c r="B48" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C48">
         <v>0</v>
       </c>
       <c r="D48">
-        <v>43</v>
+        <v>42.4</v>
       </c>
       <c r="E48">
         <v>5</v>
@@ -1230,16 +1230,16 @@
         <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C49">
         <v>0</v>
       </c>
       <c r="D49">
-        <v>8.7</v>
+        <v>12.3</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50">
@@ -1247,16 +1247,16 @@
         <v>64</v>
       </c>
       <c r="B50" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>5011041</v>
       </c>
       <c r="D50">
-        <v>76.7</v>
+        <v>48.3</v>
       </c>
       <c r="E50">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51">
@@ -1270,10 +1270,10 @@
         <v>0</v>
       </c>
       <c r="D51">
-        <v>70.9</v>
+        <v>92.4</v>
       </c>
       <c r="E51">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52">
@@ -1281,13 +1281,13 @@
         <v>66</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="C52">
         <v>0</v>
       </c>
       <c r="D52">
-        <v>24.3</v>
+        <v>47.9</v>
       </c>
       <c r="E52">
         <v>4</v>
@@ -1298,13 +1298,13 @@
         <v>67</v>
       </c>
       <c r="B53" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>7758232</v>
       </c>
       <c r="D53">
-        <v>23.1</v>
+        <v>68.3</v>
       </c>
       <c r="E53">
         <v>5</v>
@@ -1315,16 +1315,16 @@
         <v>68</v>
       </c>
       <c r="B54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C54">
         <v>0</v>
       </c>
       <c r="D54">
-        <v>83.7</v>
+        <v>32.1</v>
       </c>
       <c r="E54">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55">
@@ -1332,16 +1332,16 @@
         <v>69</v>
       </c>
       <c r="B55" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C55">
         <v>0</v>
       </c>
       <c r="D55">
-        <v>95.5</v>
+        <v>59.6</v>
       </c>
       <c r="E55">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56">
@@ -1349,16 +1349,16 @@
         <v>70</v>
       </c>
       <c r="B56" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C56">
         <v>0</v>
       </c>
       <c r="D56">
-        <v>20.8</v>
+        <v>94.7</v>
       </c>
       <c r="E56">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57">
@@ -1366,16 +1366,16 @@
         <v>71</v>
       </c>
       <c r="B57" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
       <c r="D57">
-        <v>65.9</v>
+        <v>45.9</v>
       </c>
       <c r="E57">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58">
@@ -1383,16 +1383,16 @@
         <v>72</v>
       </c>
       <c r="B58" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C58">
-        <v>8218641</v>
+        <v>8703207</v>
       </c>
       <c r="D58">
-        <v>43.6</v>
+        <v>23.6</v>
       </c>
       <c r="E58">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59">
@@ -1400,16 +1400,16 @@
         <v>73</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C59">
-        <v>4725693</v>
+        <v>0</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>8.4</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60">
@@ -1417,16 +1417,16 @@
         <v>74</v>
       </c>
       <c r="B60" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C60">
-        <v>5870406</v>
+        <v>2879366</v>
       </c>
       <c r="D60">
-        <v>52.6</v>
+        <v>9.7</v>
       </c>
       <c r="E60">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -1434,16 +1434,16 @@
         <v>75</v>
       </c>
       <c r="B61" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
       <c r="D61">
-        <v>55.8</v>
+        <v>16.3</v>
       </c>
       <c r="E61">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -1451,16 +1451,16 @@
         <v>76</v>
       </c>
       <c r="B62" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="C62">
-        <v>5992383</v>
+        <v>0</v>
       </c>
       <c r="D62">
-        <v>5.2</v>
+        <v>25.6</v>
       </c>
       <c r="E62">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63">
@@ -1468,16 +1468,16 @@
         <v>77</v>
       </c>
       <c r="B63" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C63">
-        <v>3735228</v>
+        <v>0</v>
       </c>
       <c r="D63">
-        <v>57.6</v>
+        <v>49.1</v>
       </c>
       <c r="E63">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64">
@@ -1485,16 +1485,16 @@
         <v>78</v>
       </c>
       <c r="B64" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C64">
-        <v>9366225</v>
+        <v>0</v>
       </c>
       <c r="D64">
-        <v>74.5</v>
+        <v>48.3</v>
       </c>
       <c r="E64">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -1508,10 +1508,10 @@
         <v>0</v>
       </c>
       <c r="D65">
-        <v>72.6</v>
+        <v>27.1</v>
       </c>
       <c r="E65">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -1519,16 +1519,16 @@
         <v>80</v>
       </c>
       <c r="B66" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>827208</v>
       </c>
       <c r="D66">
-        <v>97.3</v>
+        <v>75.7</v>
       </c>
       <c r="E66">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -1536,16 +1536,16 @@
         <v>81</v>
       </c>
       <c r="B67" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>4724500</v>
       </c>
       <c r="D67">
-        <v>16.5</v>
+        <v>2.9</v>
       </c>
       <c r="E67">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
@@ -1553,13 +1553,13 @@
         <v>82</v>
       </c>
       <c r="B68" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="C68">
         <v>0</v>
       </c>
       <c r="D68">
-        <v>48.8</v>
+        <v>69.4</v>
       </c>
       <c r="E68">
         <v>4</v>
@@ -1570,16 +1570,16 @@
         <v>83</v>
       </c>
       <c r="B69" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C69">
         <v>0</v>
       </c>
       <c r="D69">
-        <v>89.1</v>
+        <v>48.6</v>
       </c>
       <c r="E69">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -1587,13 +1587,13 @@
         <v>84</v>
       </c>
       <c r="B70" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C70">
         <v>0</v>
       </c>
       <c r="D70">
-        <v>73.6</v>
+        <v>52.9</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -1604,16 +1604,16 @@
         <v>85</v>
       </c>
       <c r="B71" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C71">
         <v>0</v>
       </c>
       <c r="D71">
-        <v>83.7</v>
+        <v>26.2</v>
       </c>
       <c r="E71">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72">
@@ -1621,16 +1621,16 @@
         <v>86</v>
       </c>
       <c r="B72" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C72">
-        <v>9720622</v>
+        <v>0</v>
       </c>
       <c r="D72">
-        <v>74.1</v>
+        <v>4.6</v>
       </c>
       <c r="E72">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73">
@@ -1638,16 +1638,16 @@
         <v>87</v>
       </c>
       <c r="B73" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C73">
         <v>0</v>
       </c>
       <c r="D73">
-        <v>57.8</v>
+        <v>88.1</v>
       </c>
       <c r="E73">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74">
@@ -1655,16 +1655,16 @@
         <v>88</v>
       </c>
       <c r="B74" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C74">
-        <v>4761310</v>
+        <v>0</v>
       </c>
       <c r="D74">
-        <v>18.3</v>
+        <v>92.7</v>
       </c>
       <c r="E74">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75">
@@ -1672,16 +1672,16 @@
         <v>89</v>
       </c>
       <c r="B75" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C75">
-        <v>2577405</v>
+        <v>0</v>
       </c>
       <c r="D75">
-        <v>94.9</v>
+        <v>13.8</v>
       </c>
       <c r="E75">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76">
@@ -1689,16 +1689,16 @@
         <v>90</v>
       </c>
       <c r="B76" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C76">
-        <v>5018486</v>
+        <v>0</v>
       </c>
       <c r="D76">
-        <v>57.8</v>
+        <v>14.8</v>
       </c>
       <c r="E76">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
@@ -1706,16 +1706,16 @@
         <v>91</v>
       </c>
       <c r="B77" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>9210099</v>
       </c>
       <c r="D77">
-        <v>32.5</v>
+        <v>77.9</v>
       </c>
       <c r="E77">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
@@ -1723,16 +1723,16 @@
         <v>92</v>
       </c>
       <c r="B78" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C78">
         <v>0</v>
       </c>
       <c r="D78">
-        <v>83.9</v>
+        <v>88.3</v>
       </c>
       <c r="E78">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79">
@@ -1740,16 +1740,16 @@
         <v>93</v>
       </c>
       <c r="B79" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C79">
         <v>0</v>
       </c>
       <c r="D79">
-        <v>32</v>
+        <v>48.4</v>
       </c>
       <c r="E79">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80">
@@ -1757,16 +1757,16 @@
         <v>94</v>
       </c>
       <c r="B80" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C80">
         <v>0</v>
       </c>
       <c r="D80">
-        <v>93.4</v>
+        <v>39.9</v>
       </c>
       <c r="E80">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81">
@@ -1774,16 +1774,16 @@
         <v>95</v>
       </c>
       <c r="B81" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>7457285</v>
       </c>
       <c r="D81">
-        <v>68.1</v>
+        <v>18.2</v>
       </c>
       <c r="E81">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82">
@@ -1797,10 +1797,10 @@
         <v>0</v>
       </c>
       <c r="D82">
-        <v>83.4</v>
+        <v>39.5</v>
       </c>
       <c r="E82">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83">
@@ -1808,16 +1808,16 @@
         <v>97</v>
       </c>
       <c r="B83" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C83">
         <v>0</v>
       </c>
       <c r="D83">
-        <v>22.7</v>
+        <v>63.5</v>
       </c>
       <c r="E83">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84">
@@ -1825,16 +1825,16 @@
         <v>98</v>
       </c>
       <c r="B84" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>3316829</v>
       </c>
       <c r="D84">
-        <v>80.1</v>
+        <v>91.4</v>
       </c>
       <c r="E84">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85">
@@ -1842,16 +1842,16 @@
         <v>99</v>
       </c>
       <c r="B85" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C85">
         <v>0</v>
       </c>
       <c r="D85">
-        <v>76.2</v>
+        <v>78.6</v>
       </c>
       <c r="E85">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -1859,16 +1859,16 @@
         <v>100</v>
       </c>
       <c r="B86" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C86">
-        <v>1806609</v>
+        <v>0</v>
       </c>
       <c r="D86">
-        <v>3.9</v>
+        <v>93.9</v>
       </c>
       <c r="E86">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87">
@@ -1876,13 +1876,13 @@
         <v>101</v>
       </c>
       <c r="B87" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="C87">
         <v>0</v>
       </c>
       <c r="D87">
-        <v>77.3</v>
+        <v>27.8</v>
       </c>
       <c r="E87">
         <v>4</v>
@@ -1893,16 +1893,16 @@
         <v>102</v>
       </c>
       <c r="B88" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C88">
         <v>0</v>
       </c>
       <c r="D88">
-        <v>8.8</v>
+        <v>54.4</v>
       </c>
       <c r="E88">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89">
@@ -1910,16 +1910,16 @@
         <v>103</v>
       </c>
       <c r="B89" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C89">
         <v>0</v>
       </c>
       <c r="D89">
-        <v>45</v>
+        <v>49.9</v>
       </c>
       <c r="E89">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90">
@@ -1927,16 +1927,16 @@
         <v>104</v>
       </c>
       <c r="B90" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C90">
         <v>0</v>
       </c>
       <c r="D90">
-        <v>25.3</v>
+        <v>77</v>
       </c>
       <c r="E90">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91">
@@ -1944,16 +1944,16 @@
         <v>105</v>
       </c>
       <c r="B91" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="C91">
         <v>0</v>
       </c>
       <c r="D91">
-        <v>28.7</v>
+        <v>87.1</v>
       </c>
       <c r="E91">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92">
@@ -1961,16 +1961,16 @@
         <v>106</v>
       </c>
       <c r="B92" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C92">
         <v>0</v>
       </c>
       <c r="D92">
-        <v>37.2</v>
+        <v>71.6</v>
       </c>
       <c r="E92">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93">
@@ -1978,16 +1978,16 @@
         <v>107</v>
       </c>
       <c r="B93" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C93">
         <v>0</v>
       </c>
       <c r="D93">
-        <v>29.7</v>
+        <v>57.5</v>
       </c>
       <c r="E93">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94">
@@ -1995,16 +1995,16 @@
         <v>108</v>
       </c>
       <c r="B94" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C94">
         <v>0</v>
       </c>
       <c r="D94">
-        <v>47.9</v>
+        <v>92.7</v>
       </c>
       <c r="E94">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95">
@@ -2012,16 +2012,16 @@
         <v>109</v>
       </c>
       <c r="B95" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C95">
         <v>0</v>
       </c>
       <c r="D95">
-        <v>7.6</v>
+        <v>64.1</v>
       </c>
       <c r="E95">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96">
@@ -2029,16 +2029,16 @@
         <v>110</v>
       </c>
       <c r="B96" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C96">
         <v>0</v>
       </c>
       <c r="D96">
-        <v>4.2</v>
+        <v>35.7</v>
       </c>
       <c r="E96">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97">
@@ -2046,16 +2046,16 @@
         <v>111</v>
       </c>
       <c r="B97" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C97">
-        <v>5479948</v>
+        <v>6031267</v>
       </c>
       <c r="D97">
-        <v>96.6</v>
+        <v>88.4</v>
       </c>
       <c r="E97">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98">
@@ -2063,13 +2063,13 @@
         <v>112</v>
       </c>
       <c r="B98" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C98">
-        <v>6352263</v>
+        <v>1609123</v>
       </c>
       <c r="D98">
-        <v>85.5</v>
+        <v>34</v>
       </c>
       <c r="E98">
         <v>4</v>
@@ -2080,16 +2080,16 @@
         <v>113</v>
       </c>
       <c r="B99" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C99">
         <v>0</v>
       </c>
       <c r="D99">
-        <v>44.6</v>
+        <v>62.8</v>
       </c>
       <c r="E99">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
@@ -2097,16 +2097,16 @@
         <v>114</v>
       </c>
       <c r="B100" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C100">
         <v>0</v>
       </c>
       <c r="D100">
-        <v>29.3</v>
+        <v>46.4</v>
       </c>
       <c r="E100">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101">
@@ -2114,16 +2114,16 @@
         <v>115</v>
       </c>
       <c r="B101" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C101">
         <v>0</v>
       </c>
       <c r="D101">
-        <v>61.7</v>
+        <v>28.2</v>
       </c>
       <c r="E101">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>